<commit_message>
Affichage objectifs, correction affichage pins, début PathFinder
</commit_message>
<xml_diff>
--- a/Backlogs/MiniTramways-Backlog-26.11.21.xlsx
+++ b/Backlogs/MiniTramways-Backlog-26.11.21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubRepos\MiniTramways\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B05F921-D6D4-4D36-A837-5356433D8965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D0426D-DAB6-41F8-8E7F-D9B3BE28C967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F765A07-F6B4-4E3C-A596-2A823F0537A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1F765A07-F6B4-4E3C-A596-2A823F0537A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
   <si>
     <t>Carte et bâtiments</t>
   </si>
@@ -327,6 +327,12 @@
   </si>
   <si>
     <t>Gestion de la satisfaction</t>
+  </si>
+  <si>
+    <t>Génération progressive bâtiments</t>
+  </si>
+  <si>
+    <t>29:3,21,22</t>
   </si>
 </sst>
 </file>
@@ -385,7 +391,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,9 +629,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -636,6 +639,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -648,11 +653,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,14 +976,14 @@
   <dimension ref="A2:V62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="45.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" style="4" customWidth="1"/>
@@ -991,28 +997,28 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="35" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="35" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="36"/>
+      <c r="I3" s="37"/>
     </row>
     <row r="4" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="24"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="35" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="24"/>
@@ -1025,70 +1031,70 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="41" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="41" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
       <c r="C7" s="18"/>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="42">
         <v>1.0131944444444445</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="41" t="s">
         <v>84</v>
       </c>
       <c r="H7" s="17" t="s">
@@ -1101,10 +1107,10 @@
     <row r="8" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="30" t="s">
         <v>88</v>
       </c>
       <c r="F8" s="17" t="s">
@@ -1117,16 +1123,16 @@
       <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="30" t="s">
         <v>69</v>
       </c>
       <c r="F9" s="17" t="s">
@@ -1139,19 +1145,19 @@
       <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="29" t="s">
         <v>91</v>
       </c>
       <c r="G10" s="43" t="s">
@@ -1161,24 +1167,28 @@
       <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="17"/>
       <c r="G11" s="18"/>
       <c r="H11" s="17"/>
       <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="33" t="s">
+      <c r="B12" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="32" t="s">
         <v>3</v>
       </c>
       <c r="F12" s="17"/>
@@ -1189,10 +1199,10 @@
     <row r="13" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="30" t="s">
         <v>74</v>
       </c>
       <c r="F13" s="17"/>
@@ -1203,10 +1213,10 @@
     <row r="14" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
       <c r="C14" s="20"/>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="30" t="s">
         <v>75</v>
       </c>
       <c r="F14" s="17"/>
@@ -1217,10 +1227,10 @@
     <row r="15" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
-      <c r="D15" s="34">
+      <c r="D15" s="33">
         <v>17</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="30" t="s">
         <v>76</v>
       </c>
       <c r="F15" s="17"/>
@@ -1231,10 +1241,10 @@
     <row r="16" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="30" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="17"/>
@@ -1245,8 +1255,8 @@
     <row r="17" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="17"/>
       <c r="G17" s="18"/>
       <c r="H17" s="17"/>
@@ -1255,8 +1265,8 @@
     <row r="18" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="33" t="s">
+      <c r="D18" s="29"/>
+      <c r="E18" s="32" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="17"/>
@@ -1267,10 +1277,10 @@
     <row r="19" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="17"/>
       <c r="C19" s="18"/>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="30" t="s">
         <v>31</v>
       </c>
       <c r="F19" s="17"/>
@@ -1281,10 +1291,10 @@
     <row r="20" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="30" t="s">
         <v>78</v>
       </c>
       <c r="F20" s="17"/>
@@ -1294,10 +1304,10 @@
     </row>
     <row r="21" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="21"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="22"/>
-      <c r="F21" s="28"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="22"/>
       <c r="H21" s="21"/>
       <c r="I21" s="22"/>
@@ -1314,18 +1324,18 @@
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="37" t="s">
+      <c r="C27" s="39"/>
+      <c r="D27" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="37" t="s">
+      <c r="E27" s="39"/>
+      <c r="F27" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="38"/>
+      <c r="G27" s="39"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
@@ -1405,18 +1415,18 @@
       <c r="A37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="37" t="s">
+      <c r="C37" s="39"/>
+      <c r="D37" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="37" t="s">
+      <c r="E37" s="39"/>
+      <c r="F37" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="38"/>
+      <c r="G37" s="39"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="13"/>

</xml_diff>